<commit_message>
Updating documentation for v1.1.0 of the UV-5R.
</commit_message>
<xml_diff>
--- a/Documents/Radio Configuration Table UV-5R.xlsx
+++ b/Documents/Radio Configuration Table UV-5R.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelnetherway/GitWorkspace/UV-5R/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B41E8E-AC28-154C-B4EE-7AB6D0A031C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F1AF25-D661-F447-8D23-F607A724DAE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{2F353EC1-3109-4D44-9297-7AF6286BFB6D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="1" xr2:uid="{2F353EC1-3109-4D44-9297-7AF6286BFB6D}"/>
   </bookViews>
   <sheets>
     <sheet name="v1.0.0" sheetId="1" r:id="rId1"/>
+    <sheet name="v1.1.0" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="31">
   <si>
     <t>Frequency</t>
   </si>
@@ -99,6 +100,33 @@
   </si>
   <si>
     <t>High</t>
+  </si>
+  <si>
+    <t>LF1</t>
+  </si>
+  <si>
+    <t>LF2</t>
+  </si>
+  <si>
+    <t>LF3</t>
+  </si>
+  <si>
+    <t>LF4</t>
+  </si>
+  <si>
+    <t>LF5</t>
+  </si>
+  <si>
+    <t>LF6</t>
+  </si>
+  <si>
+    <t>LF7</t>
+  </si>
+  <si>
+    <t>LF8</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
 </sst>
 </file>
@@ -143,7 +171,70 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="42">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -221,28 +312,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9342197A-6855-3B4C-A36B-604B959961DA}" name="Table1" displayName="Table1" ref="B2:T23" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9342197A-6855-3B4C-A36B-604B959961DA}" name="Table1" displayName="Table1" ref="B2:T23" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="B2:T23" xr:uid="{C17D325A-F6CF-6E45-9E03-FE14ECED045B}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{0F0DC48D-C7E9-2A46-9DC7-3682F15B042D}" name="Location" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{7603A102-6E5C-B04B-9B6F-F26375C8A809}" name="Name" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{D51AFB5A-8923-D343-A4F7-DDFA3918C662}" name="Frequency" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{D1223C4B-F031-E24C-9688-0321238B20B5}" name="Duplex" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{2E00CBBA-E069-034F-9DC4-8BF666A00DF6}" name="Offset" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{A6FDE082-7974-BA41-BFB8-5A9A12C6D07E}" name="Tone" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{FFE6335B-DC58-F94B-AB2C-8E23EAB1DBAC}" name="rToneFreq" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{90515244-BB70-0A42-9A2F-C54C8FC54C1A}" name="cToneFreq" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{0F4818F0-2E06-E346-97C5-C49340C88242}" name="DtcsCode" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{44EDBCB0-85A9-9948-8B6D-B9E561A84C27}" name="DtcsPolarity" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{CA847C26-C577-DB42-83D4-EFD10E64EBEA}" name="Mode" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{5A376B5B-76D9-F64A-9ACF-EB6D64657AE3}" name="TStep" dataDxfId="9"/>
-    <tableColumn id="19" xr3:uid="{F0B0C53A-4E20-664F-9850-FF26529352BC}" name="Power" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{81B663FC-DA31-F04F-BAA9-4D3C64225DEE}" name="Skip" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{72F0A697-99B8-5745-88BE-BDE0C988CF0F}" name="Comment" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{DA27DEA7-3387-934B-83C4-0B303EF79DD1}" name="URCALL" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{A24B1DFA-03D0-534B-BA02-4BB0F5916144}" name="RPT1CALL" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{94278AE7-9F61-F443-8905-2766BA862444}" name="RPT2CALL" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{3CB3454E-0AFE-2145-8612-3D407DE21899}" name="DVCODE" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{0F0DC48D-C7E9-2A46-9DC7-3682F15B042D}" name="Location" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{7603A102-6E5C-B04B-9B6F-F26375C8A809}" name="Name" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{D51AFB5A-8923-D343-A4F7-DDFA3918C662}" name="Frequency" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{D1223C4B-F031-E24C-9688-0321238B20B5}" name="Duplex" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{2E00CBBA-E069-034F-9DC4-8BF666A00DF6}" name="Offset" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{A6FDE082-7974-BA41-BFB8-5A9A12C6D07E}" name="Tone" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{FFE6335B-DC58-F94B-AB2C-8E23EAB1DBAC}" name="rToneFreq" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{90515244-BB70-0A42-9A2F-C54C8FC54C1A}" name="cToneFreq" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{0F4818F0-2E06-E346-97C5-C49340C88242}" name="DtcsCode" dataDxfId="31"/>
+    <tableColumn id="10" xr3:uid="{44EDBCB0-85A9-9948-8B6D-B9E561A84C27}" name="DtcsPolarity" dataDxfId="30"/>
+    <tableColumn id="11" xr3:uid="{CA847C26-C577-DB42-83D4-EFD10E64EBEA}" name="Mode" dataDxfId="29"/>
+    <tableColumn id="12" xr3:uid="{5A376B5B-76D9-F64A-9ACF-EB6D64657AE3}" name="TStep" dataDxfId="28"/>
+    <tableColumn id="19" xr3:uid="{F0B0C53A-4E20-664F-9850-FF26529352BC}" name="Power" dataDxfId="27"/>
+    <tableColumn id="13" xr3:uid="{81B663FC-DA31-F04F-BAA9-4D3C64225DEE}" name="Skip" dataDxfId="26"/>
+    <tableColumn id="14" xr3:uid="{72F0A697-99B8-5745-88BE-BDE0C988CF0F}" name="Comment" dataDxfId="25"/>
+    <tableColumn id="15" xr3:uid="{DA27DEA7-3387-934B-83C4-0B303EF79DD1}" name="URCALL" dataDxfId="24"/>
+    <tableColumn id="16" xr3:uid="{A24B1DFA-03D0-534B-BA02-4BB0F5916144}" name="RPT1CALL" dataDxfId="23"/>
+    <tableColumn id="17" xr3:uid="{94278AE7-9F61-F443-8905-2766BA862444}" name="RPT2CALL" dataDxfId="22"/>
+    <tableColumn id="18" xr3:uid="{3CB3454E-0AFE-2145-8612-3D407DE21899}" name="DVCODE" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A35C8064-2C76-1741-8D6D-007C7AE794EF}" name="Table2" displayName="Table2" ref="B2:T10" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="B2:T10" xr:uid="{03D48D7C-A000-1E46-B6BB-418101329904}"/>
+  <tableColumns count="19">
+    <tableColumn id="1" xr3:uid="{DC76DF2C-1854-B149-BA13-48EF14F94411}" name="Location" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{B6654602-8492-7241-8E02-D27F8AABD411}" name="Name" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{6CD54839-5F38-4645-A304-FC949F49AD0B}" name="Frequency" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{0290EE6A-9A94-E645-AB7E-A10F786E33B7}" name="Duplex" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{287F5C26-4BAA-3949-8D55-A149745CDC30}" name="Offset" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{1531338C-3A3D-6443-AF01-A54F320D1C2A}" name="Tone" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{3102D285-4DD4-D74C-8568-AC0A061B5C80}" name="rToneFreq" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{ED1E9804-BF0F-604D-A125-454365AAF4E1}" name="cToneFreq" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{11D5D276-5AFF-5F4D-AA7E-FA65B57749BD}" name="DtcsCode" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{B1052BDB-D80B-C844-9EFD-F5C50CB97F1A}" name="DtcsPolarity" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{9BCA39F8-E4FD-B143-A5FF-E33B00752993}" name="Mode" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{E999DEED-6531-D84D-9658-CB64495344D5}" name="TStep" dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{4FBBBDF6-DE8E-4741-8886-5542B5AD5EC6}" name="Power" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{80BBB55D-9F71-6C40-A2BF-D64CC876D749}" name="Skip" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{118D24B4-9D6D-4E40-8232-61F48D3F2F86}" name="Comment" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{518AE64F-A3AC-5E44-9CDA-64B769ABACC5}" name="URCALL" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{8E2B87FA-C515-8748-8790-1D7551E2BD11}" name="RPT1CALL" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{EF49AF01-0F26-9141-8171-88D1F314F819}" name="RPT2CALL" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{DDECAFA5-E3B7-454D-B253-022558573AD4}" name="DVCODE" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -547,7 +666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462E0174-0307-0C48-97DD-F4613CE40FD8}">
   <dimension ref="B2:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -1498,4 +1617,444 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C10B9412-18EF-8C49-AB6A-5D98372D5E9F}">
+  <dimension ref="B2:T10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1">
+        <v>446.00625000000002</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I3" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J3" s="1">
+        <v>23</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="1">
+        <v>5</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1">
+        <v>446.01875000000001</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J4" s="1">
+        <v>23</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="1">
+        <v>5</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1">
+        <v>446.03125</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>23</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="1">
+        <v>5</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1">
+        <v>446.04374999999999</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I6" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J6" s="1">
+        <v>23</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="1">
+        <v>5</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1">
+        <v>446.05624999999998</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I7" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J7" s="1">
+        <v>23</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="1">
+        <v>5</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1">
+        <v>446.06875000000002</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I8" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J8" s="1">
+        <v>23</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="1">
+        <v>5</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1">
+        <v>446.08125000000001</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I9" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J9" s="1">
+        <v>23</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="1">
+        <v>5</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="1">
+        <v>446.09375</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I10" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J10" s="1">
+        <v>23</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="1">
+        <v>5</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>